<commit_message>
Amelioration code C 3.4
</commit_message>
<xml_diff>
--- a/PlanningGRP3.xlsx
+++ b/PlanningGRP3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baptiste\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baptiste\Desktop\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D859CB9E-AC8A-43C7-8EA8-082B3DC79D7D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93D1E7-B7CC-4EB0-8006-7B7D4D7662A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{5486202A-E26D-4B4B-B52B-BB5D5C8B5EF6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="31">
   <si>
     <t>Tâches</t>
   </si>
@@ -555,7 +555,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,7 +711,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -770,7 +770,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -804,7 +804,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1140,7 +1140,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="8"/>
       <c r="H34" s="3"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1156,7 +1156,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="4"/>
       <c r="I35" s="3"/>
       <c r="J35" s="4"/>

</xml_diff>